<commit_message>
Removed USB to UART bridge, added VDDA decoupling, adjusted MCU pinout and updated spreadsheet
</commit_message>
<xml_diff>
--- a/docs/Golf GPS Pinout.xlsx
+++ b/docs/Golf GPS Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjkuh\Projects\gitRepos\golf-gps\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E817489-BEB8-42F4-88A6-55F9A5440E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAA9A74-645E-4486-A5FA-DC125EA1BD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
   <si>
     <t>Type</t>
   </si>
@@ -203,12 +203,6 @@
     <t>BOOT0</t>
   </si>
   <si>
-    <t>USART2_TX</t>
-  </si>
-  <si>
-    <t>USART2_RX</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -297,6 +291,24 @@
   </si>
   <si>
     <t>SPI3_MOSI</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>BAT_LIFE</t>
+  </si>
+  <si>
+    <t>USB_DM</t>
+  </si>
+  <si>
+    <t>USB_DP</t>
+  </si>
+  <si>
+    <t>USB_D-</t>
+  </si>
+  <si>
+    <t>USB_D+</t>
   </si>
 </sst>
 </file>
@@ -334,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +356,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,13 +515,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -512,10 +524,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -527,56 +545,6 @@
   </cellStyles>
   <dxfs count="24">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -637,13 +605,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -654,6 +615,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -701,6 +669,89 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -742,42 +793,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -879,13 +897,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -902,6 +913,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -953,7 +971,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5B02BB6-5B3E-4876-8D07-8992549633FE}" name="Table1" displayName="Table1" ref="B3:F35" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5B02BB6-5B3E-4876-8D07-8992549633FE}" name="Table1" displayName="Table1" ref="B3:F35" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B3:F35" xr:uid="{B5B02BB6-5B3E-4876-8D07-8992549633FE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -966,39 +984,39 @@
     <tableColumn id="2" xr3:uid="{8E66A8D5-5C6E-4166-9038-FEF26BCD01FC}" name="Pin Name" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{D071212A-38F4-4D5B-B66B-4FCEBBE0B1D3}" name="Type" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{DF522437-00A4-4BBC-9C31-C6D18BC0CA17}" name="Function" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{BB746511-BB98-4E01-A8D4-DE84FCFFF31A}" name="Net Name" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{BB746511-BB98-4E01-A8D4-DE84FCFFF31A}" name="Net Name" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A68771B-DCBA-4B18-A27B-10E713110357}" name="Table2" displayName="Table2" ref="H3:J11" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A68771B-DCBA-4B18-A27B-10E713110357}" name="Table2" displayName="Table2" ref="H3:J11" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="H3:J11" xr:uid="{0A68771B-DCBA-4B18-A27B-10E713110357}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{21ECF538-2A63-46A6-88F0-B4531AEFE31D}" name="Pin Number" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{237E0112-A0CA-49B1-8E56-468A06EC4D72}" name="Pin Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{4701401A-63BF-4F8C-90EF-E76890BB7F4B}" name="Net Name" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{21ECF538-2A63-46A6-88F0-B4531AEFE31D}" name="Pin Number" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{237E0112-A0CA-49B1-8E56-468A06EC4D72}" name="Pin Name" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4701401A-63BF-4F8C-90EF-E76890BB7F4B}" name="Net Name" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B8550477-14BD-4B25-AA85-550B9D3DB429}" name="Table24" displayName="Table24" ref="L3:N12" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B8550477-14BD-4B25-AA85-550B9D3DB429}" name="Table24" displayName="Table24" ref="L3:N12" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="L3:N12" xr:uid="{B8550477-14BD-4B25-AA85-550B9D3DB429}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{044628D4-1D7B-4F92-949E-5358BB89B11C}" name="Pin Number" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D50AEAC2-FB72-4131-91A1-F796FBB28A48}" name="Pin Name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{842A792F-1225-473A-880F-2CE7812ABF89}" name="Net Name" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{044628D4-1D7B-4F92-949E-5358BB89B11C}" name="Pin Number" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D50AEAC2-FB72-4131-91A1-F796FBB28A48}" name="Pin Name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{842A792F-1225-473A-880F-2CE7812ABF89}" name="Net Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1269,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,20 +1307,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="H2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="B2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="H2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
       <c r="L2" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
@@ -1350,7 +1368,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
@@ -1360,19 +1378,19 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="L4" s="3">
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -1395,18 +1413,18 @@
         <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>44</v>
       </c>
       <c r="L5" s="3">
         <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1430,18 +1448,18 @@
         <v>3</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L6" s="3">
         <v>3</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N6" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1453,7 +1471,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
@@ -1463,9 +1481,9 @@
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>34</v>
       </c>
       <c r="L7" s="3">
@@ -1474,7 +1492,7 @@
       <c r="M7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1486,28 +1504,26 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="F8" s="15"/>
       <c r="H8" s="3">
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>53</v>
       </c>
       <c r="L8" s="3">
         <v>5</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N8" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="N8" s="12" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1518,18 +1534,22 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="16" t="s">
-        <v>80</v>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="H9" s="3">
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>51</v>
       </c>
       <c r="L9" s="3">
@@ -1538,7 +1558,7 @@
       <c r="M9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="N9" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1552,24 +1572,24 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H10" s="3">
         <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="L10" s="3">
         <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" s="10" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1581,13 +1601,11 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H11" s="4">
         <v>8</v>
@@ -1595,17 +1613,17 @@
       <c r="I11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="L11" s="4">
         <v>8</v>
       </c>
       <c r="M11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -1616,21 +1634,19 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="L12" s="4">
         <v>9</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="N12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1642,7 +1658,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
@@ -1657,9 +1673,9 @@
         <v>13</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="16"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -1670,11 +1686,11 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -1685,7 +1701,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
@@ -1700,7 +1716,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
@@ -1716,7 +1732,7 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1728,7 +1744,7 @@
         <v>39</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
@@ -1743,7 +1759,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
@@ -1759,8 +1775,8 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="16" t="s">
-        <v>80</v>
+      <c r="F21" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1771,10 +1787,10 @@
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>42</v>
@@ -1788,10 +1804,10 @@
         <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>43</v>
@@ -1804,12 +1820,14 @@
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
-        <v>44</v>
+      <c r="D24" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -1819,12 +1837,14 @@
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>38</v>
+      <c r="D25" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -1834,9 +1854,9 @@
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>45</v>
@@ -1849,9 +1869,9 @@
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>46</v>
@@ -1864,10 +1884,10 @@
       <c r="C28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16" t="s">
-        <v>80</v>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -1878,13 +1898,13 @@
         <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -1895,13 +1915,13 @@
         <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -1911,12 +1931,14 @@
       <c r="C31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="E31" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -1927,7 +1949,7 @@
         <v>27</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
@@ -1944,7 +1966,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -1955,7 +1977,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>54</v>
@@ -1972,7 +1994,7 @@
         <v>39</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">

</xml_diff>

<commit_message>
Updated pinout and spreadsheet, PCB changes
</commit_message>
<xml_diff>
--- a/docs/Golf GPS Pinout.xlsx
+++ b/docs/Golf GPS Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjkuh\Projects\gitRepos\golf-gps\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAA9A74-645E-4486-A5FA-DC125EA1BD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D550C3A0-8CB1-40FD-A52E-C73131D56EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
   <si>
     <t>Type</t>
   </si>
@@ -489,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,16 +527,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1288,7 +1285,7 @@
   <dimension ref="B2:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,23 +1304,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="H2" s="14" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="H2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="L2" s="14" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="L2" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
     </row>
     <row r="3" spans="2:14" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -1507,7 +1504,7 @@
         <v>57</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="13"/>
       <c r="H8" s="3">
         <v>5</v>
       </c>
@@ -1730,7 +1727,9 @@
       <c r="C18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="9" t="s">
         <v>47</v>
@@ -1820,13 +1819,13 @@
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1837,13 +1836,13 @@
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1854,7 +1853,7 @@
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="15"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="1" t="s">
         <v>59</v>
       </c>
@@ -1869,7 +1868,7 @@
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="15"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="1" t="s">
         <v>60</v>
       </c>

</xml_diff>